<commit_message>
batch import files and stations
</commit_message>
<xml_diff>
--- a/app/public/static/aktemp-stations-template.xlsx
+++ b/app/public/static/aktemp-stations-template.xlsx
@@ -1,63 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeff/git/ecosheds/aktemp/app/public/static/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7F6AF9D1-9297-2145-A14D-E74116A6E46F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E4849BB-B449-B940-8CEE-09FCC38300A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300"/>
+    <workbookView xWindow="-25600" yWindow="500" windowWidth="25600" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
-    <sheet name="TABLE" sheetId="2" r:id="rId2"/>
+    <sheet name="STATIONS" sheetId="2" r:id="rId2"/>
+    <sheet name="EXAMPLES" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="76">
-  <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>description</t>
-  </si>
-  <si>
-    <t>latitude</t>
-  </si>
-  <si>
-    <t>longitude</t>
-  </si>
-  <si>
-    <t>placement</t>
-  </si>
-  <si>
-    <t>timezone</t>
-  </si>
-  <si>
-    <t>waterbody_name</t>
-  </si>
-  <si>
-    <t>waterbody_type</t>
-  </si>
-  <si>
-    <t>active</t>
-  </si>
-  <si>
-    <t>mixed</t>
-  </si>
-  <si>
-    <t>reference</t>
-  </si>
-  <si>
-    <t>private</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="72">
   <si>
     <t>MAIN</t>
   </si>
@@ -74,18 +51,9 @@
     <t>LAKE</t>
   </si>
   <si>
-    <t>SITE 001</t>
-  </si>
-  <si>
     <t>SITE 002</t>
   </si>
   <si>
-    <t>SITE 003</t>
-  </si>
-  <si>
-    <t>UNKNOWN</t>
-  </si>
-  <si>
     <t>https://nwis.waterdata.usgs.gov/…</t>
   </si>
   <si>
@@ -95,33 +63,18 @@
     <t>Echo Lake</t>
   </si>
   <si>
-    <t>AKTEMP Stations Table Template</t>
-  </si>
-  <si>
     <t>Updated:</t>
   </si>
   <si>
     <t>Description:</t>
   </si>
   <si>
-    <t>Spreadsheet template to generate stations table for batch importing into AKTEMP</t>
-  </si>
-  <si>
     <t>Instructions:</t>
   </si>
   <si>
-    <t>1. Read column descriptions and requirements below</t>
-  </si>
-  <si>
-    <t>4. Click submit to save stations (or fix validation errors, if any)</t>
-  </si>
-  <si>
     <t>Columns:</t>
   </si>
   <si>
-    <t>Station Code</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -149,87 +102,39 @@
     <t>Well-mixed</t>
   </si>
   <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <t>Private</t>
   </si>
   <si>
     <t>X</t>
   </si>
   <si>
-    <t>must be unique within an organization</t>
-  </si>
-  <si>
     <t>max 250 characters</t>
   </si>
   <si>
-    <t>between 4-50 characters</t>
-  </si>
-  <si>
     <t>decimal degrees</t>
   </si>
   <si>
-    <t>decimal degrees (negative since AK is west of central meridian)</t>
-  </si>
-  <si>
     <t>decimal between -90 and 90</t>
   </si>
   <si>
     <t>decimal between -180 and 180</t>
   </si>
   <si>
-    <t>'US/Alaska' or 'US/Pacific'</t>
-  </si>
-  <si>
     <t>local timezone of station</t>
   </si>
   <si>
-    <t>'MAIN', 'SIDE', 'UNKNOWN'</t>
-  </si>
-  <si>
-    <t>location within channel (Main Channel or Side Channel)</t>
-  </si>
-  <si>
     <t>name of waterbody</t>
   </si>
   <si>
-    <t>type of waterbody</t>
-  </si>
-  <si>
-    <t>indicates if station is actively monitored</t>
-  </si>
-  <si>
-    <t>indicates if station is located within well-mixed portion of the waterbody</t>
-  </si>
-  <si>
     <t>URL to external data source (e.g., Inletkeeper, USGS NWIS)</t>
   </si>
   <si>
-    <t xml:space="preserve">indicates if station and associated data should be kept private. </t>
-  </si>
-  <si>
-    <t>'TRUE', 'FALSE', 'UNKNOWN'</t>
-  </si>
-  <si>
-    <t>'TRUE', 'FALSE'</t>
-  </si>
-  <si>
-    <t>'STREAM', 'LAKE', 'OTHER', 'UNKNOWN'</t>
-  </si>
-  <si>
     <t>valid URL</t>
   </si>
   <si>
     <t>narrative description of the station location (e.g., relative to roads or other geographic features)</t>
   </si>
   <si>
-    <t>Column Name</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -245,17 +150,117 @@
     <t>OTHER</t>
   </si>
   <si>
-    <t>2. Fill out stations on TABLE sheet</t>
-  </si>
-  <si>
-    <t>3. Copy and paste station rows (excluding header row) from TABLE to the Stations Batch Import table in AKTEMP</t>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>Reference URL</t>
+  </si>
+  <si>
+    <t>Mining Canal near Fairbanks</t>
+  </si>
+  <si>
+    <t>Echo Lake near center</t>
+  </si>
+  <si>
+    <t>ECHO</t>
+  </si>
+  <si>
+    <t>Definitions:</t>
+  </si>
+  <si>
+    <t>1. Read column descriptions and definitions below (note that definitions of various options are defined below the Columns table) and review example file configurations on EXAMPLES sheet</t>
+  </si>
+  <si>
+    <t>2. Fill out stations on STATIONS sheet</t>
+  </si>
+  <si>
+    <t>3. Copy and paste station rows (excluding header row) from STATIONS to the Stations Batch Import table in AKTEMP</t>
+  </si>
+  <si>
+    <t>5. Fix any validation or other errors that are reported (if any), and click Submit to try again.</t>
+  </si>
+  <si>
+    <t>4. Click submit to save stations to AKTEMP</t>
+  </si>
+  <si>
+    <t>between 1-50 characters</t>
+  </si>
+  <si>
+    <t>brief name or ID of that station. must be unique within an organization.</t>
+  </si>
+  <si>
+    <t>decimal degrees (should be negative since AK is west of central meridian)</t>
+  </si>
+  <si>
+    <t>US/Alaska, US/Pacific</t>
+  </si>
+  <si>
+    <t>Placement:</t>
+  </si>
+  <si>
+    <t>main channel</t>
+  </si>
+  <si>
+    <t>side channel</t>
+  </si>
+  <si>
+    <t>location within channel (main channel or side channel). See definitions below.
+leave blank if unknown or not applicable (e.g., station is in a lake)</t>
+  </si>
+  <si>
+    <t>MAIN, SIDE</t>
+  </si>
+  <si>
+    <t>TRUE, FALSE</t>
+  </si>
+  <si>
+    <t>indicates if station is located within well-mixed portion of the waterbody. leave blank if unknown.</t>
+  </si>
+  <si>
+    <t>indicates if station and associated data should be kept private and not appear on the public data explorer</t>
+  </si>
+  <si>
+    <t>STREAM, LAKE, OTHER</t>
+  </si>
+  <si>
+    <t>type of waterbody. leave blank if unknown.</t>
+  </si>
+  <si>
+    <t>indicates if station is actively monitored. leave blank if unknown. leave blank if unknown.</t>
+  </si>
+  <si>
+    <t>Waterbody Type:</t>
+  </si>
+  <si>
+    <t>free-flowing stream or river</t>
+  </si>
+  <si>
+    <t>lake or pond</t>
+  </si>
+  <si>
+    <t>wetlands, or man-made channel</t>
+  </si>
+  <si>
+    <t>Template and instructions for creating stations table for batch importing into AKTEMP</t>
+  </si>
+  <si>
+    <t>Column</t>
+  </si>
+  <si>
+    <t>AKTEMP Batch Import Stations Template</t>
+  </si>
+  <si>
+    <t>max 50 characters</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="25" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+  </numFmts>
+  <fonts count="26" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -444,6 +449,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -632,7 +645,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -756,6 +769,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -802,7 +914,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -815,15 +927,6 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -839,6 +942,57 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -900,7 +1054,83 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -916,80 +1146,6 @@
         <scheme val="minor"/>
       </font>
     </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1004,14 +1160,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B12:F24" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="B12:F24"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="Column Name" dataDxfId="6"/>
-    <tableColumn id="2" name="Label" dataDxfId="5"/>
-    <tableColumn id="3" name="Required" dataDxfId="4"/>
-    <tableColumn id="4" name="Allowed Values" dataDxfId="3"/>
-    <tableColumn id="5" name="Notes" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B13:E25" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5" tableBorderDxfId="4">
+  <autoFilter ref="B13:E25" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="4">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Column" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Required" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Allowed Values" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1313,307 +1468,321 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="39" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="93.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="93.5" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="24" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3">
-        <v>44692</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="B3" s="21">
+        <v>44812</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
       <c r="B4" s="3"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
       <c r="B6" s="4"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="37" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5"/>
       <c r="B8" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="5"/>
       <c r="B10" s="4" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="5"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="C13" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="26"/>
+      <c r="D15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A16" s="5"/>
+      <c r="B16" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A17" s="5"/>
+      <c r="B17" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="A18" s="5"/>
+      <c r="B18" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C18" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="40" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="B19" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="26"/>
+      <c r="D19" s="29" t="s">
+        <v>57</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="B20" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="26"/>
+      <c r="D20" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="B21" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="26"/>
+      <c r="D21" s="29" t="s">
+        <v>61</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="B22" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="26"/>
+      <c r="D22" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="40" x14ac:dyDescent="0.25">
+      <c r="B23" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="26"/>
+      <c r="D23" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="20" x14ac:dyDescent="0.25">
+      <c r="B24" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="26"/>
+      <c r="D24" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="27" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="3" t="s">
+    <row r="25" spans="1:5" ht="40" x14ac:dyDescent="0.25">
+      <c r="B25" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="14" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+      <c r="C28" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="18"/>
+      <c r="C30" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="20"/>
+      <c r="C31" s="31" t="s">
+        <v>37</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C19" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D20" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C21" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D21" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D22" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E22" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B7:E7"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1622,172 +1791,257 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="E44" sqref="E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="13.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="10.83203125" style="10"/>
+    <col min="1" max="1" width="10.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="K2" s="9"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD5184F-52B3-EF46-AA5F-BE0833D74299}">
+  <dimension ref="A1:L4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.6640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40" style="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="7"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2" s="8">
+        <v>61.5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>-152.38200000000001</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="G2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I2" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="C1" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="13" t="s">
+      <c r="K2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="8">
+        <v>62.23</v>
+      </c>
+      <c r="D3" s="8">
+        <v>-151.23099999999999</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L3" s="8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="8">
+        <v>63.98</v>
+      </c>
+      <c r="D4" s="8">
+        <v>-153.42099999999999</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="14" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="14" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="C2" s="11">
-        <v>61.5</v>
-      </c>
-      <c r="D2" s="11">
-        <v>-152.38200000000001</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="11">
-        <v>62.23</v>
-      </c>
-      <c r="D3" s="11">
-        <v>-151.23099999999999</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="11" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="11" t="b">
+      <c r="I4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="L3" s="11" t="b">
+      <c r="J4" s="8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="11">
-        <v>63.98</v>
-      </c>
-      <c r="D4" s="11">
-        <v>-153.42099999999999</v>
-      </c>
-      <c r="E4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="H4" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" s="11" t="b">
-        <v>0</v>
-      </c>
-      <c r="L4" s="11" t="b">
+      <c r="L4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{31D4F587-408C-5540-A8E2-FBA868C42EEB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>